<commit_message>
Launching at the cluster
</commit_message>
<xml_diff>
--- a/Session3/comparacion_conf_spatial_pyramid.xlsx
+++ b/Session3/comparacion_conf_spatial_pyramid.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="22">
   <si>
     <t>2x2</t>
   </si>
@@ -66,6 +66,30 @@
   </si>
   <si>
     <t>Running time</t>
+  </si>
+  <si>
+    <t>1x3 depth 2</t>
+  </si>
+  <si>
+    <t>2x2 depth 2</t>
+  </si>
+  <si>
+    <t>86.3371 (3.6781)</t>
+  </si>
+  <si>
+    <t>85.3271 (2.9752)</t>
+  </si>
+  <si>
+    <t>P-value</t>
+  </si>
+  <si>
+    <t>T-test</t>
+  </si>
+  <si>
+    <t>1x2 depth 2</t>
+  </si>
+  <si>
+    <t>85.0079 (2.8188)</t>
   </si>
 </sst>
 </file>
@@ -178,26 +202,26 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -512,113 +536,122 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:K19"/>
+  <dimension ref="B1:N19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I18" sqref="I18"/>
+      <selection activeCell="N19" sqref="N19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="E1" s="6" t="s">
+    <row r="1" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="E1" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="F1" s="6"/>
-      <c r="G1" s="5" t="s">
+      <c r="F1" s="11"/>
+      <c r="G1" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="H1" s="5"/>
-      <c r="I1" s="8" t="s">
+      <c r="H1" s="12"/>
+      <c r="I1" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="J1" s="8"/>
-    </row>
-    <row r="2" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B2" s="4" t="s">
+      <c r="J1" s="13"/>
+    </row>
+    <row r="2" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B2" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="C2" s="4"/>
-      <c r="D2" s="4"/>
-      <c r="E2" s="4">
+      <c r="C2" s="9"/>
+      <c r="D2" s="9"/>
+      <c r="E2" s="9">
         <v>48.379600000000003</v>
       </c>
-      <c r="F2" s="4"/>
-      <c r="G2" s="4">
+      <c r="F2" s="9"/>
+      <c r="G2" s="9">
         <v>1.2522</v>
       </c>
-      <c r="H2" s="4"/>
-      <c r="I2" s="4">
+      <c r="H2" s="9"/>
+      <c r="I2" s="9">
         <v>207</v>
       </c>
-      <c r="J2" s="4"/>
-    </row>
-    <row r="5" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B5" s="7" t="s">
+      <c r="J2" s="9"/>
+    </row>
+    <row r="5" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B5" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="C5" s="7"/>
-      <c r="D5" s="7"/>
-      <c r="E5" s="7"/>
-      <c r="F5" s="7"/>
-      <c r="G5" s="7"/>
-      <c r="H5" s="7"/>
-      <c r="I5" s="7"/>
-      <c r="J5" s="7"/>
-      <c r="K5" s="7"/>
-    </row>
-    <row r="6" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B6" s="13"/>
-      <c r="C6" s="6" t="s">
+      <c r="C5" s="10"/>
+      <c r="D5" s="10"/>
+      <c r="E5" s="10"/>
+      <c r="F5" s="10"/>
+      <c r="G5" s="10"/>
+      <c r="H5" s="10"/>
+      <c r="I5" s="10"/>
+      <c r="J5" s="10"/>
+      <c r="K5" s="10"/>
+    </row>
+    <row r="6" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B6" s="8"/>
+      <c r="C6" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="D6" s="6"/>
-      <c r="E6" s="6"/>
-      <c r="F6" s="5" t="s">
+      <c r="D6" s="11"/>
+      <c r="E6" s="11"/>
+      <c r="F6" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="G6" s="5"/>
-      <c r="H6" s="5"/>
-      <c r="I6" s="8" t="s">
+      <c r="G6" s="12"/>
+      <c r="H6" s="12"/>
+      <c r="I6" s="13" t="s">
         <v>6</v>
       </c>
-      <c r="J6" s="8"/>
-      <c r="K6" s="8"/>
-    </row>
-    <row r="7" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B7" s="12" t="s">
+      <c r="J6" s="13"/>
+      <c r="K6" s="13"/>
+      <c r="M6" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="7" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B7" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="C7" s="9" t="s">
+      <c r="C7" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="D7" s="10" t="s">
+      <c r="D7" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="E7" s="11" t="s">
+      <c r="E7" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="F7" s="9" t="s">
+      <c r="F7" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="G7" s="10" t="s">
+      <c r="G7" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="H7" s="11" t="s">
+      <c r="H7" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="I7" s="9" t="s">
+      <c r="I7" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="J7" s="10" t="s">
+      <c r="J7" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="K7" s="11" t="s">
+      <c r="K7" s="6" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="8" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B8" s="12">
+      <c r="M7" t="s">
+        <v>15</v>
+      </c>
+      <c r="N7" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="8" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B8" s="7">
         <v>2</v>
       </c>
       <c r="C8" s="1">
@@ -648,9 +681,15 @@
       <c r="K8" s="3">
         <v>1487</v>
       </c>
-    </row>
-    <row r="9" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B9" s="12">
+      <c r="M8" t="s">
+        <v>14</v>
+      </c>
+      <c r="N8" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="9" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B9" s="7">
         <v>3</v>
       </c>
       <c r="C9" s="1">
@@ -680,73 +719,102 @@
       <c r="K9" s="3">
         <v>2532</v>
       </c>
-    </row>
-    <row r="12" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B12" s="7" t="s">
+      <c r="M9" t="s">
+        <v>18</v>
+      </c>
+      <c r="N9">
+        <v>0.89004749999999999</v>
+      </c>
+    </row>
+    <row r="11" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="M11" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="12" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B12" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="C12" s="7"/>
-      <c r="D12" s="7"/>
-      <c r="E12" s="7"/>
-      <c r="F12" s="7"/>
-      <c r="G12" s="7"/>
-      <c r="H12" s="7"/>
-      <c r="I12" s="7"/>
-      <c r="J12" s="7"/>
-      <c r="K12" s="7"/>
-    </row>
-    <row r="13" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B13" s="13"/>
-      <c r="C13" s="6" t="s">
+      <c r="C12" s="10"/>
+      <c r="D12" s="10"/>
+      <c r="E12" s="10"/>
+      <c r="F12" s="10"/>
+      <c r="G12" s="10"/>
+      <c r="H12" s="10"/>
+      <c r="I12" s="10"/>
+      <c r="J12" s="10"/>
+      <c r="K12" s="10"/>
+      <c r="M12" t="s">
+        <v>15</v>
+      </c>
+      <c r="N12" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="13" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B13" s="8"/>
+      <c r="C13" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="D13" s="6"/>
-      <c r="E13" s="6"/>
-      <c r="F13" s="5" t="s">
+      <c r="D13" s="11"/>
+      <c r="E13" s="11"/>
+      <c r="F13" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="G13" s="5"/>
-      <c r="H13" s="5"/>
-      <c r="I13" s="8" t="s">
+      <c r="G13" s="12"/>
+      <c r="H13" s="12"/>
+      <c r="I13" s="13" t="s">
         <v>6</v>
       </c>
-      <c r="J13" s="8"/>
-      <c r="K13" s="8"/>
-    </row>
-    <row r="14" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B14" s="12" t="s">
+      <c r="J13" s="13"/>
+      <c r="K13" s="13"/>
+      <c r="M13" t="s">
+        <v>20</v>
+      </c>
+      <c r="N13" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="14" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B14" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="C14" s="9" t="s">
+      <c r="C14" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="D14" s="10" t="s">
+      <c r="D14" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="E14" s="11" t="s">
+      <c r="E14" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="F14" s="9" t="s">
+      <c r="F14" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="G14" s="10" t="s">
+      <c r="G14" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="H14" s="11" t="s">
+      <c r="H14" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="I14" s="9" t="s">
+      <c r="I14" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="J14" s="10" t="s">
+      <c r="J14" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="K14" s="11" t="s">
+      <c r="K14" s="6" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="15" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B15" s="12">
+      <c r="M14" t="s">
+        <v>18</v>
+      </c>
+      <c r="N14">
+        <v>0.84969519999999998</v>
+      </c>
+    </row>
+    <row r="15" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B15" s="7">
         <v>2</v>
       </c>
       <c r="C15" s="1">
@@ -777,8 +845,8 @@
         <v>782</v>
       </c>
     </row>
-    <row r="16" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B16" s="12">
+    <row r="16" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B16" s="7">
         <v>3</v>
       </c>
       <c r="C16" s="1">
@@ -816,17 +884,17 @@
     </row>
   </sheetData>
   <mergeCells count="15">
-    <mergeCell ref="B2:D2"/>
-    <mergeCell ref="B12:K12"/>
-    <mergeCell ref="C13:E13"/>
-    <mergeCell ref="F13:H13"/>
-    <mergeCell ref="I13:K13"/>
     <mergeCell ref="E1:F1"/>
     <mergeCell ref="G1:H1"/>
     <mergeCell ref="I1:J1"/>
     <mergeCell ref="E2:F2"/>
     <mergeCell ref="G2:H2"/>
     <mergeCell ref="I2:J2"/>
+    <mergeCell ref="B2:D2"/>
+    <mergeCell ref="B12:K12"/>
+    <mergeCell ref="C13:E13"/>
+    <mergeCell ref="F13:H13"/>
+    <mergeCell ref="I13:K13"/>
     <mergeCell ref="C6:E6"/>
     <mergeCell ref="F6:H6"/>
     <mergeCell ref="I6:K6"/>

</xml_diff>